<commit_message>
finished all phase 1 categorizations, except google
</commit_message>
<xml_diff>
--- a/Overall Error and Accuracy.xlsx
+++ b/Overall Error and Accuracy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrissoria/Documents/Research/Categorization_AI_experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA82DB69-EB8C-4649-82B1-9EAB9DD337E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535C9E2A-EE03-7F4C-9274-91DB08FF110C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4060" yWindow="3160" windowWidth="27240" windowHeight="16440" xr2:uid="{241983BD-D857-8348-9A37-C778D09AF26C}"/>
+    <workbookView xWindow="0" yWindow="3120" windowWidth="27240" windowHeight="16440" xr2:uid="{241983BD-D857-8348-9A37-C778D09AF26C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -431,7 +431,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,6 +506,9 @@
       <c r="D4" s="1">
         <v>0</v>
       </c>
+      <c r="F4" s="2">
+        <v>2.5000000000000001E-3</v>
+      </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -518,6 +521,9 @@
       <c r="D5" s="1">
         <v>0</v>
       </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -529,6 +535,9 @@
       <c r="D6" s="1">
         <v>0</v>
       </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -537,7 +546,12 @@
       <c r="B7" s="2">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -549,6 +563,9 @@
       <c r="D8" s="2">
         <v>7.4999999999999997E-3</v>
       </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -559,6 +576,9 @@
       </c>
       <c r="D9" s="2">
         <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>